<commit_message>
Work on report generation
</commit_message>
<xml_diff>
--- a/public/sample-files/Eval Uploadables - factors.xlsx
+++ b/public/sample-files/Eval Uploadables - factors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>short_hand</t>
   </si>
@@ -171,15 +171,6 @@
     <t>Lab Learning Experience</t>
   </si>
   <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>Please disregard this. This does not play any part in the analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ii </t>
-  </si>
-  <si>
     <t>Irresponsibility Indicator</t>
   </si>
   <si>
@@ -193,6 +184,9 @@
   </si>
   <si>
     <t>quantiative measure of the teaching and course administration excellence</t>
+  </si>
+  <si>
+    <t>ii</t>
   </si>
 </sst>
 </file>
@@ -999,9 +993,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1194,6 +1190,9 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
         <v>50</v>
       </c>
       <c r="C18" t="s">
@@ -1209,17 +1208,6 @@
       </c>
       <c r="C19" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>